<commit_message>
:memo: add template for cell resonator data
</commit_message>
<xml_diff>
--- a/tests/data/sample_missing/sample_sheet_nosensor.xlsx
+++ b/tests/data/sample_missing/sample_sheet_nosensor.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7C6856-9F42-5D4C-A1A8-D2B620B72632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B96AEAB-5763-FF42-BE44-D080941D3136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5500" yWindow="1860" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3323,7 +3323,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>